<commit_message>
created _old folder containing all old defaults models to be rebuilt
</commit_message>
<xml_diff>
--- a/doc/concepts/conceptual_models.xlsx
+++ b/doc/concepts/conceptual_models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\doc\concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD3F7DD-4A02-4DD8-AEB8-023681F0AD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC96C4C-408D-4380-80D2-A61502B04EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="887" activeTab="3" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="887" activeTab="8" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="28" r:id="rId1"/>
@@ -2622,6 +2622,13 @@
     <xf numFmtId="169" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="4" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2669,13 +2676,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4085,22 +4085,22 @@
       </c>
     </row>
     <row r="6" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="151" t="s">
         <v>274</v>
       </c>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="151"/>
+      <c r="O6" s="151"/>
       <c r="P6" s="55"/>
       <c r="R6" s="103" t="s">
         <v>263</v>
@@ -4110,20 +4110,20 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="148"/>
-      <c r="C7" s="148"/>
-      <c r="D7" s="148"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
-      <c r="K7" s="148"/>
-      <c r="L7" s="148"/>
-      <c r="M7" s="148"/>
-      <c r="N7" s="148"/>
-      <c r="O7" s="148"/>
+      <c r="B7" s="151"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
+      <c r="L7" s="151"/>
+      <c r="M7" s="151"/>
+      <c r="N7" s="151"/>
+      <c r="O7" s="151"/>
       <c r="P7" s="55"/>
       <c r="R7" s="104"/>
       <c r="S7" s="55" t="s">
@@ -4135,37 +4135,37 @@
       </c>
     </row>
     <row r="8" spans="2:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="148"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="148"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="148"/>
-      <c r="K8" s="148"/>
-      <c r="L8" s="148"/>
-      <c r="M8" s="148"/>
-      <c r="N8" s="148"/>
-      <c r="O8" s="148"/>
+      <c r="B8" s="151"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="151"/>
+      <c r="I8" s="151"/>
+      <c r="J8" s="151"/>
+      <c r="K8" s="151"/>
+      <c r="L8" s="151"/>
+      <c r="M8" s="151"/>
+      <c r="N8" s="151"/>
+      <c r="O8" s="151"/>
       <c r="P8" s="55"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
+      <c r="B9" s="151"/>
+      <c r="C9" s="151"/>
+      <c r="D9" s="151"/>
+      <c r="E9" s="151"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="151"/>
+      <c r="K9" s="151"/>
+      <c r="L9" s="151"/>
+      <c r="M9" s="151"/>
+      <c r="N9" s="151"/>
+      <c r="O9" s="151"/>
       <c r="P9" s="55"/>
       <c r="R9" s="106"/>
       <c r="S9" s="55" t="s">
@@ -4177,37 +4177,37 @@
       </c>
     </row>
     <row r="10" spans="2:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="148"/>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="148"/>
+      <c r="B10" s="151"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="151"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="151"/>
+      <c r="K10" s="151"/>
+      <c r="L10" s="151"/>
+      <c r="M10" s="151"/>
+      <c r="N10" s="151"/>
+      <c r="O10" s="151"/>
       <c r="P10" s="55"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="148"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="148"/>
-      <c r="I11" s="148"/>
-      <c r="J11" s="148"/>
-      <c r="K11" s="148"/>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
-      <c r="N11" s="148"/>
-      <c r="O11" s="148"/>
+      <c r="B11" s="151"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="151"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="151"/>
+      <c r="M11" s="151"/>
+      <c r="N11" s="151"/>
+      <c r="O11" s="151"/>
       <c r="P11" s="55"/>
       <c r="V11" s="108"/>
       <c r="W11" s="109" t="s">
@@ -4282,13 +4282,13 @@
       <c r="P19" s="55"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="153" t="s">
         <v>286</v>
       </c>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="151"/>
+      <c r="C20" s="153"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="154"/>
       <c r="G20" s="116" t="s">
         <v>298</v>
       </c>
@@ -4298,11 +4298,11 @@
       <c r="K20" s="57"/>
       <c r="L20" s="57"/>
       <c r="M20" s="118"/>
-      <c r="N20" s="152" t="s">
+      <c r="N20" s="155" t="s">
         <v>299</v>
       </c>
-      <c r="O20" s="150"/>
-      <c r="P20" s="151"/>
+      <c r="O20" s="153"/>
+      <c r="P20" s="154"/>
       <c r="Q20" s="125" t="s">
         <v>293</v>
       </c>
@@ -4325,49 +4325,49 @@
       <c r="B22" s="55" t="s">
         <v>287</v>
       </c>
-      <c r="G22" s="147" t="s">
+      <c r="G22" s="150" t="s">
         <v>294</v>
       </c>
-      <c r="H22" s="148"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="148"/>
-      <c r="K22" s="148"/>
-      <c r="L22" s="148"/>
-      <c r="M22" s="149"/>
-      <c r="N22" s="144" t="s">
+      <c r="H22" s="151"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="151"/>
+      <c r="K22" s="151"/>
+      <c r="L22" s="151"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="147" t="s">
         <v>261</v>
       </c>
-      <c r="O22" s="145"/>
-      <c r="P22" s="146"/>
+      <c r="O22" s="148"/>
+      <c r="P22" s="149"/>
       <c r="Q22" s="55" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="23" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="147"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
-      <c r="K23" s="148"/>
-      <c r="L23" s="148"/>
-      <c r="M23" s="149"/>
+      <c r="G23" s="150"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="151"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="152"/>
       <c r="N23" s="128"/>
       <c r="O23" s="115"/>
       <c r="P23" s="126"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="G24" s="147"/>
-      <c r="H24" s="148"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="148"/>
-      <c r="K24" s="148"/>
-      <c r="L24" s="148"/>
-      <c r="M24" s="149"/>
-      <c r="N24" s="144" t="s">
+      <c r="G24" s="150"/>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="151"/>
+      <c r="K24" s="151"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="147" t="s">
         <v>275</v>
       </c>
-      <c r="O24" s="145"/>
-      <c r="P24" s="146"/>
+      <c r="O24" s="148"/>
+      <c r="P24" s="149"/>
       <c r="Q24" s="55" t="s">
         <v>301</v>
       </c>
@@ -4406,20 +4406,20 @@
       <c r="B27" s="55" t="s">
         <v>288</v>
       </c>
-      <c r="G27" s="147" t="s">
+      <c r="G27" s="150" t="s">
         <v>296</v>
       </c>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="148"/>
-      <c r="L27" s="148"/>
-      <c r="M27" s="149"/>
-      <c r="N27" s="144" t="s">
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="152"/>
+      <c r="N27" s="147" t="s">
         <v>295</v>
       </c>
-      <c r="O27" s="145"/>
-      <c r="P27" s="146"/>
+      <c r="O27" s="148"/>
+      <c r="P27" s="149"/>
     </row>
     <row r="28" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="120"/>
@@ -4455,113 +4455,113 @@
       <c r="B30" s="55" t="s">
         <v>289</v>
       </c>
-      <c r="G30" s="147" t="s">
+      <c r="G30" s="150" t="s">
         <v>297</v>
       </c>
-      <c r="H30" s="148"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="148"/>
-      <c r="K30" s="148"/>
-      <c r="L30" s="148"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="144" t="s">
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="151"/>
+      <c r="K30" s="151"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="152"/>
+      <c r="N30" s="147" t="s">
         <v>276</v>
       </c>
-      <c r="O30" s="145"/>
-      <c r="P30" s="146"/>
+      <c r="O30" s="148"/>
+      <c r="P30" s="149"/>
       <c r="Q30" s="55" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="31" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="147"/>
-      <c r="H31" s="148"/>
-      <c r="I31" s="148"/>
-      <c r="J31" s="148"/>
-      <c r="K31" s="148"/>
-      <c r="L31" s="148"/>
-      <c r="M31" s="149"/>
+      <c r="G31" s="150"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="151"/>
+      <c r="J31" s="151"/>
+      <c r="K31" s="151"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="152"/>
       <c r="N31" s="128"/>
       <c r="O31" s="115"/>
       <c r="P31" s="126"/>
     </row>
     <row r="32" spans="2:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="147"/>
-      <c r="H32" s="148"/>
-      <c r="I32" s="148"/>
-      <c r="J32" s="148"/>
-      <c r="K32" s="148"/>
-      <c r="L32" s="148"/>
-      <c r="M32" s="149"/>
-      <c r="N32" s="144" t="s">
+      <c r="G32" s="150"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="151"/>
+      <c r="K32" s="151"/>
+      <c r="L32" s="151"/>
+      <c r="M32" s="152"/>
+      <c r="N32" s="147" t="s">
         <v>277</v>
       </c>
-      <c r="O32" s="145"/>
-      <c r="P32" s="146"/>
-      <c r="Q32" s="148" t="s">
+      <c r="O32" s="148"/>
+      <c r="P32" s="149"/>
+      <c r="Q32" s="151" t="s">
         <v>303</v>
       </c>
-      <c r="R32" s="148"/>
-      <c r="S32" s="148"/>
-      <c r="T32" s="148"/>
-      <c r="U32" s="148"/>
-      <c r="V32" s="148"/>
-      <c r="W32" s="148"/>
-      <c r="X32" s="148"/>
+      <c r="R32" s="151"/>
+      <c r="S32" s="151"/>
+      <c r="T32" s="151"/>
+      <c r="U32" s="151"/>
+      <c r="V32" s="151"/>
+      <c r="W32" s="151"/>
+      <c r="X32" s="151"/>
       <c r="Y32" s="117"/>
     </row>
     <row r="33" spans="2:25" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="147"/>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="148"/>
-      <c r="K33" s="148"/>
-      <c r="L33" s="148"/>
-      <c r="M33" s="149"/>
+      <c r="G33" s="150"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="151"/>
+      <c r="K33" s="151"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="152"/>
       <c r="N33" s="128"/>
       <c r="O33" s="115"/>
       <c r="P33" s="126"/>
-      <c r="Q33" s="148"/>
-      <c r="R33" s="148"/>
-      <c r="S33" s="148"/>
-      <c r="T33" s="148"/>
-      <c r="U33" s="148"/>
-      <c r="V33" s="148"/>
-      <c r="W33" s="148"/>
-      <c r="X33" s="148"/>
+      <c r="Q33" s="151"/>
+      <c r="R33" s="151"/>
+      <c r="S33" s="151"/>
+      <c r="T33" s="151"/>
+      <c r="U33" s="151"/>
+      <c r="V33" s="151"/>
+      <c r="W33" s="151"/>
+      <c r="X33" s="151"/>
       <c r="Y33" s="117"/>
     </row>
     <row r="34" spans="2:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="147"/>
-      <c r="H34" s="148"/>
-      <c r="I34" s="148"/>
-      <c r="J34" s="148"/>
-      <c r="K34" s="148"/>
-      <c r="L34" s="148"/>
-      <c r="M34" s="149"/>
-      <c r="N34" s="144" t="s">
+      <c r="G34" s="150"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="151"/>
+      <c r="K34" s="151"/>
+      <c r="L34" s="151"/>
+      <c r="M34" s="152"/>
+      <c r="N34" s="147" t="s">
         <v>278</v>
       </c>
-      <c r="O34" s="145"/>
-      <c r="P34" s="146"/>
-      <c r="Q34" s="148"/>
-      <c r="R34" s="148"/>
-      <c r="S34" s="148"/>
-      <c r="T34" s="148"/>
-      <c r="U34" s="148"/>
-      <c r="V34" s="148"/>
-      <c r="W34" s="148"/>
-      <c r="X34" s="148"/>
+      <c r="O34" s="148"/>
+      <c r="P34" s="149"/>
+      <c r="Q34" s="151"/>
+      <c r="R34" s="151"/>
+      <c r="S34" s="151"/>
+      <c r="T34" s="151"/>
+      <c r="U34" s="151"/>
+      <c r="V34" s="151"/>
+      <c r="W34" s="151"/>
+      <c r="X34" s="151"/>
       <c r="Y34" s="117"/>
     </row>
     <row r="35" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G35" s="147"/>
-      <c r="H35" s="148"/>
-      <c r="I35" s="148"/>
-      <c r="J35" s="148"/>
-      <c r="K35" s="148"/>
-      <c r="L35" s="148"/>
-      <c r="M35" s="149"/>
+      <c r="G35" s="150"/>
+      <c r="H35" s="151"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="151"/>
+      <c r="K35" s="151"/>
+      <c r="L35" s="151"/>
+      <c r="M35" s="152"/>
       <c r="N35" s="128"/>
       <c r="O35" s="115"/>
       <c r="P35" s="126"/>
@@ -4576,18 +4576,18 @@
       <c r="Y35" s="117"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="G36" s="147"/>
-      <c r="H36" s="148"/>
-      <c r="I36" s="148"/>
-      <c r="J36" s="148"/>
-      <c r="K36" s="148"/>
-      <c r="L36" s="148"/>
-      <c r="M36" s="149"/>
-      <c r="N36" s="144" t="s">
+      <c r="G36" s="150"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="151"/>
+      <c r="K36" s="151"/>
+      <c r="L36" s="151"/>
+      <c r="M36" s="152"/>
+      <c r="N36" s="147" t="s">
         <v>279</v>
       </c>
-      <c r="O36" s="145"/>
-      <c r="P36" s="146"/>
+      <c r="O36" s="148"/>
+      <c r="P36" s="149"/>
       <c r="Q36" s="55" t="s">
         <v>304</v>
       </c>
@@ -4629,21 +4629,21 @@
       <c r="G39" s="119" t="s">
         <v>305</v>
       </c>
-      <c r="N39" s="144" t="s">
+      <c r="N39" s="147" t="s">
         <v>280</v>
       </c>
-      <c r="O39" s="145"/>
-      <c r="P39" s="146"/>
-      <c r="Q39" s="148" t="s">
+      <c r="O39" s="148"/>
+      <c r="P39" s="149"/>
+      <c r="Q39" s="151" t="s">
         <v>306</v>
       </c>
-      <c r="R39" s="148"/>
-      <c r="S39" s="148"/>
-      <c r="T39" s="148"/>
-      <c r="U39" s="148"/>
-      <c r="V39" s="148"/>
-      <c r="W39" s="148"/>
-      <c r="X39" s="148"/>
+      <c r="R39" s="151"/>
+      <c r="S39" s="151"/>
+      <c r="T39" s="151"/>
+      <c r="U39" s="151"/>
+      <c r="V39" s="151"/>
+      <c r="W39" s="151"/>
+      <c r="X39" s="151"/>
     </row>
     <row r="40" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="120"/>
@@ -4682,21 +4682,21 @@
       <c r="G42" s="119" t="s">
         <v>307</v>
       </c>
-      <c r="N42" s="144" t="s">
+      <c r="N42" s="147" t="s">
         <v>281</v>
       </c>
-      <c r="O42" s="145"/>
-      <c r="P42" s="146"/>
-      <c r="Q42" s="148" t="s">
+      <c r="O42" s="148"/>
+      <c r="P42" s="149"/>
+      <c r="Q42" s="151" t="s">
         <v>308</v>
       </c>
-      <c r="R42" s="148"/>
-      <c r="S42" s="148"/>
-      <c r="T42" s="148"/>
-      <c r="U42" s="148"/>
-      <c r="V42" s="148"/>
-      <c r="W42" s="148"/>
-      <c r="X42" s="148"/>
+      <c r="R42" s="151"/>
+      <c r="S42" s="151"/>
+      <c r="T42" s="151"/>
+      <c r="U42" s="151"/>
+      <c r="V42" s="151"/>
+      <c r="W42" s="151"/>
+      <c r="X42" s="151"/>
     </row>
     <row r="43" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N43" s="128"/>
@@ -4704,21 +4704,21 @@
       <c r="P43" s="126"/>
     </row>
     <row r="44" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N44" s="144" t="s">
+      <c r="N44" s="147" t="s">
         <v>282</v>
       </c>
-      <c r="O44" s="145"/>
-      <c r="P44" s="146"/>
-      <c r="Q44" s="153" t="s">
+      <c r="O44" s="148"/>
+      <c r="P44" s="149"/>
+      <c r="Q44" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="R44" s="153"/>
-      <c r="S44" s="153"/>
-      <c r="T44" s="153"/>
-      <c r="U44" s="153"/>
-      <c r="V44" s="153"/>
-      <c r="W44" s="153"/>
-      <c r="X44" s="153"/>
+      <c r="R44" s="156"/>
+      <c r="S44" s="156"/>
+      <c r="T44" s="156"/>
+      <c r="U44" s="156"/>
+      <c r="V44" s="156"/>
+      <c r="W44" s="156"/>
+      <c r="X44" s="156"/>
     </row>
     <row r="45" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="128"/>
@@ -4726,21 +4726,21 @@
       <c r="P45" s="126"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="N46" s="144" t="s">
+      <c r="N46" s="147" t="s">
         <v>283</v>
       </c>
-      <c r="O46" s="145"/>
-      <c r="P46" s="146"/>
-      <c r="Q46" s="148" t="s">
+      <c r="O46" s="148"/>
+      <c r="P46" s="149"/>
+      <c r="Q46" s="151" t="s">
         <v>310</v>
       </c>
-      <c r="R46" s="148"/>
-      <c r="S46" s="148"/>
-      <c r="T46" s="148"/>
-      <c r="U46" s="148"/>
-      <c r="V46" s="148"/>
-      <c r="W46" s="148"/>
-      <c r="X46" s="148"/>
+      <c r="R46" s="151"/>
+      <c r="S46" s="151"/>
+      <c r="T46" s="151"/>
+      <c r="U46" s="151"/>
+      <c r="V46" s="151"/>
+      <c r="W46" s="151"/>
+      <c r="X46" s="151"/>
     </row>
     <row r="47" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N47" s="128"/>
@@ -4748,21 +4748,21 @@
       <c r="P47" s="126"/>
     </row>
     <row r="48" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N48" s="144" t="s">
+      <c r="N48" s="147" t="s">
         <v>284</v>
       </c>
-      <c r="O48" s="145"/>
-      <c r="P48" s="146"/>
-      <c r="Q48" s="148" t="s">
+      <c r="O48" s="148"/>
+      <c r="P48" s="149"/>
+      <c r="Q48" s="151" t="s">
         <v>311</v>
       </c>
-      <c r="R48" s="148"/>
-      <c r="S48" s="148"/>
-      <c r="T48" s="148"/>
-      <c r="U48" s="148"/>
-      <c r="V48" s="148"/>
-      <c r="W48" s="148"/>
-      <c r="X48" s="148"/>
+      <c r="R48" s="151"/>
+      <c r="S48" s="151"/>
+      <c r="T48" s="151"/>
+      <c r="U48" s="151"/>
+      <c r="V48" s="151"/>
+      <c r="W48" s="151"/>
+      <c r="X48" s="151"/>
     </row>
     <row r="49" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="120"/>
@@ -4801,75 +4801,75 @@
       <c r="G51" s="119" t="s">
         <v>312</v>
       </c>
-      <c r="N51" s="144" t="s">
+      <c r="N51" s="147" t="s">
         <v>314</v>
       </c>
-      <c r="O51" s="145"/>
-      <c r="P51" s="146"/>
-      <c r="Q51" s="148" t="s">
+      <c r="O51" s="148"/>
+      <c r="P51" s="149"/>
+      <c r="Q51" s="151" t="s">
         <v>315</v>
       </c>
-      <c r="R51" s="148"/>
-      <c r="S51" s="148"/>
-      <c r="T51" s="148"/>
-      <c r="U51" s="148"/>
-      <c r="V51" s="148"/>
-      <c r="W51" s="148"/>
-      <c r="X51" s="148"/>
+      <c r="R51" s="151"/>
+      <c r="S51" s="151"/>
+      <c r="T51" s="151"/>
+      <c r="U51" s="151"/>
+      <c r="V51" s="151"/>
+      <c r="W51" s="151"/>
+      <c r="X51" s="151"/>
     </row>
     <row r="52" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="N53" s="144" t="s">
+      <c r="N53" s="147" t="s">
         <v>341</v>
       </c>
-      <c r="O53" s="145"/>
-      <c r="P53" s="146"/>
-      <c r="Q53" s="148" t="s">
+      <c r="O53" s="148"/>
+      <c r="P53" s="149"/>
+      <c r="Q53" s="151" t="s">
         <v>344</v>
       </c>
-      <c r="R53" s="148"/>
-      <c r="S53" s="148"/>
-      <c r="T53" s="148"/>
-      <c r="U53" s="148"/>
-      <c r="V53" s="148"/>
-      <c r="W53" s="148"/>
-      <c r="X53" s="148"/>
+      <c r="R53" s="151"/>
+      <c r="S53" s="151"/>
+      <c r="T53" s="151"/>
+      <c r="U53" s="151"/>
+      <c r="V53" s="151"/>
+      <c r="W53" s="151"/>
+      <c r="X53" s="151"/>
     </row>
     <row r="54" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="N55" s="144" t="s">
+      <c r="N55" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="O55" s="145"/>
-      <c r="P55" s="146"/>
-      <c r="Q55" s="148" t="s">
+      <c r="O55" s="148"/>
+      <c r="P55" s="149"/>
+      <c r="Q55" s="151" t="s">
         <v>345</v>
       </c>
-      <c r="R55" s="148"/>
-      <c r="S55" s="148"/>
-      <c r="T55" s="148"/>
-      <c r="U55" s="148"/>
-      <c r="V55" s="148"/>
-      <c r="W55" s="148"/>
-      <c r="X55" s="148"/>
+      <c r="R55" s="151"/>
+      <c r="S55" s="151"/>
+      <c r="T55" s="151"/>
+      <c r="U55" s="151"/>
+      <c r="V55" s="151"/>
+      <c r="W55" s="151"/>
+      <c r="X55" s="151"/>
     </row>
     <row r="56" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N57" s="144" t="s">
+      <c r="N57" s="147" t="s">
         <v>343</v>
       </c>
-      <c r="O57" s="145"/>
-      <c r="P57" s="146"/>
-      <c r="Q57" s="148" t="s">
+      <c r="O57" s="148"/>
+      <c r="P57" s="149"/>
+      <c r="Q57" s="151" t="s">
         <v>346</v>
       </c>
-      <c r="R57" s="148"/>
-      <c r="S57" s="148"/>
-      <c r="T57" s="148"/>
-      <c r="U57" s="148"/>
-      <c r="V57" s="148"/>
-      <c r="W57" s="148"/>
-      <c r="X57" s="148"/>
+      <c r="R57" s="151"/>
+      <c r="S57" s="151"/>
+      <c r="T57" s="151"/>
+      <c r="U57" s="151"/>
+      <c r="V57" s="151"/>
+      <c r="W57" s="151"/>
+      <c r="X57" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -9448,10 +9448,10 @@
       <c r="I7" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="156" t="s">
+      <c r="Q7" s="159" t="s">
         <v>83</v>
       </c>
-      <c r="R7" s="156"/>
+      <c r="R7" s="159"/>
       <c r="T7" t="s">
         <v>8</v>
       </c>
@@ -13366,19 +13366,19 @@
       <c r="A1" s="97" t="s">
         <v>285</v>
       </c>
-      <c r="V1" s="157" t="s">
+      <c r="V1" s="160" t="s">
         <v>355</v>
       </c>
-      <c r="X1" s="158" t="s">
+      <c r="X1" s="161" t="s">
         <v>348</v>
       </c>
-      <c r="Z1" s="158" t="s">
+      <c r="Z1" s="161" t="s">
         <v>349</v>
       </c>
-      <c r="AB1" s="157" t="s">
+      <c r="AB1" s="160" t="s">
         <v>352</v>
       </c>
-      <c r="AD1" s="157" t="s">
+      <c r="AD1" s="160" t="s">
         <v>337</v>
       </c>
     </row>
@@ -13405,11 +13405,11 @@
       <c r="Q2" t="s">
         <v>319</v>
       </c>
-      <c r="V2" s="157"/>
-      <c r="X2" s="158"/>
-      <c r="Z2" s="158"/>
-      <c r="AB2" s="157"/>
-      <c r="AD2" s="157"/>
+      <c r="V2" s="160"/>
+      <c r="X2" s="161"/>
+      <c r="Z2" s="161"/>
+      <c r="AB2" s="160"/>
+      <c r="AD2" s="160"/>
       <c r="AH2" t="s">
         <v>61</v>
       </c>
@@ -13472,11 +13472,11 @@
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="157"/>
-      <c r="X3" s="158"/>
-      <c r="Z3" s="158"/>
-      <c r="AB3" s="157"/>
-      <c r="AD3" s="157"/>
+      <c r="V3" s="160"/>
+      <c r="X3" s="161"/>
+      <c r="Z3" s="161"/>
+      <c r="AB3" s="160"/>
+      <c r="AD3" s="160"/>
       <c r="AH3" t="s">
         <v>3</v>
       </c>
@@ -13533,11 +13533,11 @@
       <c r="T4" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="157"/>
-      <c r="X4" s="158"/>
-      <c r="Z4" s="158"/>
-      <c r="AB4" s="157"/>
-      <c r="AD4" s="157"/>
+      <c r="V4" s="160"/>
+      <c r="X4" s="161"/>
+      <c r="Z4" s="161"/>
+      <c r="AB4" s="160"/>
+      <c r="AD4" s="160"/>
       <c r="AO4" t="s">
         <v>7</v>
       </c>
@@ -13585,11 +13585,11 @@
       <c r="T5" t="s">
         <v>188</v>
       </c>
-      <c r="V5" s="157"/>
-      <c r="X5" s="158"/>
-      <c r="Z5" s="158"/>
-      <c r="AB5" s="157"/>
-      <c r="AD5" s="157"/>
+      <c r="V5" s="160"/>
+      <c r="X5" s="161"/>
+      <c r="Z5" s="161"/>
+      <c r="AB5" s="160"/>
+      <c r="AD5" s="160"/>
     </row>
     <row r="6" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
@@ -13605,12 +13605,12 @@
       <c r="T6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="157"/>
-      <c r="X6" s="158"/>
-      <c r="Z6" s="158"/>
+      <c r="V6" s="160"/>
+      <c r="X6" s="161"/>
+      <c r="Z6" s="161"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="157"/>
-      <c r="AD6" s="159"/>
+      <c r="AB6" s="160"/>
+      <c r="AD6" s="162"/>
       <c r="AF6" s="3" t="s">
         <v>351</v>
       </c>
@@ -16453,13 +16453,13 @@
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="144" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
       <c r="G2" s="68" t="s">
         <v>257</v>
       </c>
@@ -16468,13 +16468,13 @@
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="160"/>
-      <c r="B3" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
       <c r="G3" s="68" t="s">
         <v>3</v>
       </c>
@@ -16519,13 +16519,13 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="160"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160" t="s">
+      <c r="A4" s="144"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="144" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
       <c r="O4" s="68" t="s">
         <v>7</v>
       </c>
@@ -16576,10 +16576,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="160"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160" t="s">
+      <c r="A5" s="144"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="69"/>
@@ -16619,11 +16619,11 @@
       <c r="AR5" s="69"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="160" t="s">
+      <c r="A6" s="144"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="144" t="s">
         <v>137</v>
       </c>
       <c r="G6" s="69"/>
@@ -18339,7 +18339,7 @@
   </sheetPr>
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -18400,7 +18400,7 @@
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
       <c r="K2" s="52"/>
-      <c r="L2" s="161"/>
+      <c r="L2" s="145"/>
       <c r="M2" s="52" t="s">
         <v>92</v>
       </c>
@@ -18548,10 +18548,10 @@
       <c r="H5" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="162"/>
-      <c r="J5" s="162"/>
-      <c r="K5" s="162"/>
-      <c r="L5" s="162"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="146"/>
       <c r="M5" s="52" t="s">
         <v>188</v>
       </c>
@@ -19867,23 +19867,23 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="154" t="s">
+      <c r="K31" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="L31" s="154"/>
-      <c r="M31" s="154"/>
+      <c r="L31" s="157"/>
+      <c r="M31" s="157"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="154" t="s">
+      <c r="O31" s="157" t="s">
         <v>203</v>
       </c>
-      <c r="P31" s="154"/>
-      <c r="Q31" s="154"/>
+      <c r="P31" s="157"/>
+      <c r="Q31" s="157"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="154" t="s">
+      <c r="S31" s="157" t="s">
         <v>191</v>
       </c>
-      <c r="T31" s="154"/>
-      <c r="U31" s="154"/>
+      <c r="T31" s="157"/>
+      <c r="U31" s="157"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K32" t="s">
@@ -20078,11 +20078,11 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="154" t="s">
+      <c r="K39" s="157" t="s">
         <v>193</v>
       </c>
-      <c r="L39" s="154"/>
-      <c r="M39" s="154"/>
+      <c r="L39" s="157"/>
+      <c r="M39" s="157"/>
       <c r="O39" s="3" t="s">
         <v>128</v>
       </c>
@@ -21459,17 +21459,17 @@
       <c r="P33" s="41"/>
     </row>
     <row r="34" spans="1:47" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="155" t="s">
+      <c r="J34" s="158" t="s">
         <v>194</v>
       </c>
-      <c r="K34" s="155"/>
-      <c r="L34" s="155"/>
+      <c r="K34" s="158"/>
+      <c r="L34" s="158"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="155" t="s">
+      <c r="N34" s="158" t="s">
         <v>195</v>
       </c>
-      <c r="O34" s="155"/>
-      <c r="P34" s="155"/>
+      <c r="O34" s="158"/>
+      <c r="P34" s="158"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
         <v>191</v>
@@ -21869,16 +21869,16 @@
       </c>
     </row>
     <row r="42" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="155" t="s">
+      <c r="J42" s="158" t="s">
         <v>196</v>
       </c>
-      <c r="K42" s="155"/>
-      <c r="L42" s="155"/>
-      <c r="N42" s="155" t="s">
+      <c r="K42" s="158"/>
+      <c r="L42" s="158"/>
+      <c r="N42" s="158" t="s">
         <v>201</v>
       </c>
-      <c r="O42" s="155"/>
-      <c r="P42" s="155"/>
+      <c r="O42" s="158"/>
+      <c r="P42" s="158"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
@@ -22018,14 +22018,14 @@
       </c>
     </row>
     <row r="50" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N50" s="155" t="s">
+      <c r="N50" s="158" t="s">
         <v>180</v>
       </c>
-      <c r="O50" s="155"/>
-      <c r="P50" s="155"/>
-      <c r="Q50" s="155"/>
-      <c r="R50" s="155"/>
-      <c r="S50" s="155"/>
+      <c r="O50" s="158"/>
+      <c r="P50" s="158"/>
+      <c r="Q50" s="158"/>
+      <c r="R50" s="158"/>
+      <c r="S50" s="158"/>
       <c r="X50" s="3" t="s">
         <v>128</v>
       </c>
@@ -23704,23 +23704,23 @@
       <c r="P33" s="41"/>
     </row>
     <row r="34" spans="1:47" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="155" t="s">
+      <c r="J34" s="158" t="s">
         <v>194</v>
       </c>
-      <c r="K34" s="155"/>
-      <c r="L34" s="155"/>
+      <c r="K34" s="158"/>
+      <c r="L34" s="158"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="155" t="s">
+      <c r="N34" s="158" t="s">
         <v>197</v>
       </c>
-      <c r="O34" s="155"/>
-      <c r="P34" s="155"/>
+      <c r="O34" s="158"/>
+      <c r="P34" s="158"/>
       <c r="Q34" s="3"/>
-      <c r="R34" s="155" t="s">
+      <c r="R34" s="158" t="s">
         <v>191</v>
       </c>
-      <c r="S34" s="155"/>
-      <c r="T34" s="155"/>
+      <c r="S34" s="158"/>
+      <c r="T34" s="158"/>
       <c r="X34" s="3" t="s">
         <v>176</v>
       </c>
@@ -24116,12 +24116,12 @@
       <c r="J42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="N42" s="155" t="s">
+      <c r="N42" s="158" t="s">
         <v>198</v>
       </c>
-      <c r="O42" s="155"/>
-      <c r="P42" s="155"/>
-      <c r="Q42" s="155"/>
+      <c r="O42" s="158"/>
+      <c r="P42" s="158"/>
+      <c r="Q42" s="158"/>
       <c r="X42" s="3" t="s">
         <v>128</v>
       </c>
@@ -25228,11 +25228,11 @@
       <c r="N26" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="R26" s="155" t="s">
+      <c r="R26" s="158" t="s">
         <v>190</v>
       </c>
-      <c r="S26" s="155"/>
-      <c r="T26" s="155"/>
+      <c r="S26" s="158"/>
+      <c r="T26" s="158"/>
       <c r="V26" s="3" t="s">
         <v>182</v>
       </c>
@@ -25884,17 +25884,17 @@
       <c r="P33" s="41"/>
     </row>
     <row r="34" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="155" t="s">
+      <c r="J34" s="158" t="s">
         <v>174</v>
       </c>
-      <c r="K34" s="155"/>
-      <c r="L34" s="155"/>
+      <c r="K34" s="158"/>
+      <c r="L34" s="158"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="155" t="s">
+      <c r="N34" s="158" t="s">
         <v>175</v>
       </c>
-      <c r="O34" s="155"/>
-      <c r="P34" s="155"/>
+      <c r="O34" s="158"/>
+      <c r="P34" s="158"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
         <v>191</v>
@@ -26293,16 +26293,16 @@
       </c>
     </row>
     <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="155" t="s">
+      <c r="J42" s="158" t="s">
         <v>179</v>
       </c>
-      <c r="K42" s="155"/>
-      <c r="L42" s="155"/>
-      <c r="N42" s="155" t="s">
+      <c r="K42" s="158"/>
+      <c r="L42" s="158"/>
+      <c r="N42" s="158" t="s">
         <v>200</v>
       </c>
-      <c r="O42" s="155"/>
-      <c r="P42" s="155"/>
+      <c r="O42" s="158"/>
+      <c r="P42" s="158"/>
       <c r="T42" s="3" t="s">
         <v>128</v>
       </c>
@@ -26537,14 +26537,14 @@
       </c>
     </row>
     <row r="50" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N50" s="155" t="s">
+      <c r="N50" s="158" t="s">
         <v>180</v>
       </c>
-      <c r="O50" s="155"/>
-      <c r="P50" s="155"/>
-      <c r="Q50" s="155"/>
-      <c r="R50" s="155"/>
-      <c r="S50" s="155"/>
+      <c r="O50" s="158"/>
+      <c r="P50" s="158"/>
+      <c r="Q50" s="158"/>
+      <c r="R50" s="158"/>
+      <c r="S50" s="158"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N51" s="58" t="s">
@@ -26654,11 +26654,11 @@
   </sheetPr>
   <dimension ref="A1:AZ93"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="7" topLeftCell="G41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N33" sqref="N33:N35"/>
+      <selection pane="bottomRight" activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lca concept not working
</commit_message>
<xml_diff>
--- a/doc/concepts/conceptual_models.xlsx
+++ b/doc/concepts/conceptual_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\doc\concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC96C4C-408D-4380-80D2-A61502B04EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4597E6D3-E650-41F4-86D7-858CA73F02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="887" activeTab="8" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="887" xr2:uid="{B26EA869-E077-404B-8821-28AAA0DECE59}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="28" r:id="rId1"/>
@@ -932,7 +932,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="370">
   <si>
     <t>flows</t>
   </si>
@@ -2022,6 +2022,27 @@
   </si>
   <si>
     <t>€</t>
+  </si>
+  <si>
+    <t>chi fa cosa</t>
+  </si>
+  <si>
+    <t>fatto</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>fatto (da aggiustare come funziona in pyesm, LR)</t>
+  </si>
+  <si>
+    <t>AV, VB</t>
+  </si>
+  <si>
+    <t>Invertire segni dello storage</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2058,7 @@
     <numFmt numFmtId="169" formatCode="0;\-0;\-"/>
     <numFmt numFmtId="170" formatCode="0.0;\-0.0;\-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2115,6 +2136,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2395,7 +2424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -2677,6 +2706,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4014,11 +4044,11 @@
   </sheetPr>
   <dimension ref="B1:Y57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="Q57" sqref="Q57:X57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y58" sqref="Y58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="55" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" style="55" customWidth="1"/>
@@ -4313,6 +4343,9 @@
       <c r="V20" s="57"/>
       <c r="W20" s="57"/>
       <c r="X20" s="57"/>
+      <c r="Y20" s="56" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="21" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="112"/>
@@ -4420,6 +4453,9 @@
       </c>
       <c r="O27" s="148"/>
       <c r="P27" s="149"/>
+      <c r="Y27" s="55" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="28" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="120"/>
@@ -4508,7 +4544,9 @@
       <c r="V32" s="151"/>
       <c r="W32" s="151"/>
       <c r="X32" s="151"/>
-      <c r="Y32" s="117"/>
+      <c r="Y32" s="55" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="33" spans="2:25" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="150"/>
@@ -4552,7 +4590,9 @@
       <c r="V34" s="151"/>
       <c r="W34" s="151"/>
       <c r="X34" s="151"/>
-      <c r="Y34" s="117"/>
+      <c r="Y34" s="117" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="35" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G35" s="150"/>
@@ -4590,6 +4630,9 @@
       <c r="P36" s="149"/>
       <c r="Q36" s="55" t="s">
         <v>304</v>
+      </c>
+      <c r="Y36" s="55" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4644,6 +4687,9 @@
       <c r="V39" s="151"/>
       <c r="W39" s="151"/>
       <c r="X39" s="151"/>
+      <c r="Y39" s="55" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="40" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="120"/>
@@ -4697,6 +4743,9 @@
       <c r="V42" s="151"/>
       <c r="W42" s="151"/>
       <c r="X42" s="151"/>
+      <c r="Y42" s="55" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="43" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N43" s="128"/>
@@ -4719,6 +4768,9 @@
       <c r="V44" s="156"/>
       <c r="W44" s="156"/>
       <c r="X44" s="156"/>
+      <c r="Y44" s="55" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="45" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="128"/>
@@ -4741,6 +4793,9 @@
       <c r="V46" s="151"/>
       <c r="W46" s="151"/>
       <c r="X46" s="151"/>
+      <c r="Y46" s="55" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="47" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N47" s="128"/>
@@ -4763,8 +4818,11 @@
       <c r="V48" s="151"/>
       <c r="W48" s="151"/>
       <c r="X48" s="151"/>
-    </row>
-    <row r="49" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y48" s="55" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="120"/>
       <c r="C49" s="120"/>
       <c r="D49" s="120"/>
@@ -4789,12 +4847,12 @@
       <c r="W49" s="120"/>
       <c r="X49" s="120"/>
     </row>
-    <row r="50" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N50" s="128"/>
       <c r="O50" s="115"/>
       <c r="P50" s="126"/>
     </row>
-    <row r="51" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="55" t="s">
         <v>292</v>
       </c>
@@ -4816,9 +4874,12 @@
       <c r="V51" s="151"/>
       <c r="W51" s="151"/>
       <c r="X51" s="151"/>
-    </row>
-    <row r="52" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y51" s="55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N53" s="147" t="s">
         <v>341</v>
       </c>
@@ -4834,9 +4895,12 @@
       <c r="V53" s="151"/>
       <c r="W53" s="151"/>
       <c r="X53" s="151"/>
-    </row>
-    <row r="54" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y53" s="55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N55" s="147" t="s">
         <v>342</v>
       </c>
@@ -4852,9 +4916,12 @@
       <c r="V55" s="151"/>
       <c r="W55" s="151"/>
       <c r="X55" s="151"/>
-    </row>
-    <row r="56" spans="2:24" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y55" s="55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N57" s="147" t="s">
         <v>343</v>
       </c>
@@ -4870,6 +4937,9 @@
       <c r="V57" s="151"/>
       <c r="W57" s="151"/>
       <c r="X57" s="151"/>
+      <c r="Y57" s="55" t="s">
+        <v>368</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -4937,10 +5007,10 @@
   <dimension ref="A1:AD54"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="7" ySplit="7" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA40" sqref="AA40"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4955,6 +5025,9 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="21"/>
     <col min="17" max="21" width="4.7109375" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
@@ -9248,11 +9321,11 @@
   </sheetPr>
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H24" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="7" ySplit="8" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q41" sqref="Q41:R45"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9847,7 +9920,7 @@
       </c>
       <c r="T15" s="101" cm="1">
         <f t="array" ref="T15">SUM(MMULT(M41:R45,M31:R31*_xlfn.MUNIT(6)))</f>
-        <v>21.5</v>
+        <v>27.5</v>
       </c>
       <c r="AB15" s="7">
         <v>0</v>
@@ -10273,7 +10346,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R31" s="1">
         <v>-0.5</v>
@@ -10406,6 +10479,9 @@
       <c r="M40" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="Q40" s="163" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -10436,10 +10512,10 @@
         <v>0</v>
       </c>
       <c r="Q41" s="131">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="R41" s="131">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.25">
@@ -10471,10 +10547,10 @@
         <v>6</v>
       </c>
       <c r="Q42" s="131">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="R42" s="131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.25">
@@ -10576,10 +10652,10 @@
         <v>0</v>
       </c>
       <c r="Q45" s="131">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R45" s="131">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.25">
@@ -10791,7 +10867,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomRight" activeCell="AC29" sqref="AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14855,10 +14931,10 @@
   <dimension ref="A1:AR43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
+      <selection pane="bottomRight" activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22231,7 +22307,7 @@
       <pane xSplit="4" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24613,10 +24689,10 @@
   <dimension ref="A1:AW56"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V28" sqref="V28"/>
+      <selection pane="bottomRight" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26654,11 +26730,11 @@
   </sheetPr>
   <dimension ref="A1:AZ93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G41" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U27" sqref="U27"/>
+      <selection pane="bottomRight" activeCell="AE34" sqref="AE34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>